<commit_message>
Database Change in Subject. Sql Code Included.
</commit_message>
<xml_diff>
--- a/Subject.xlsx
+++ b/Subject.xlsx
@@ -267,6 +267,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="3" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="4"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -279,7 +280,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="4"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -590,8 +590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -612,7 +612,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>19</v>
       </c>
       <c r="B2" t="s">
@@ -626,7 +626,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="4"/>
+      <c r="A3" s="5"/>
       <c r="B3" t="s">
         <v>4</v>
       </c>
@@ -638,7 +638,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="4"/>
+      <c r="A4" s="5"/>
       <c r="B4" t="s">
         <v>5</v>
       </c>
@@ -650,7 +650,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="4"/>
+      <c r="A5" s="5"/>
       <c r="B5" t="s">
         <v>6</v>
       </c>
@@ -662,7 +662,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="4"/>
+      <c r="A6" s="5"/>
       <c r="B6" t="s">
         <v>7</v>
       </c>
@@ -674,55 +674,55 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="4"/>
-      <c r="B7" s="7" t="s">
+      <c r="A7" s="5"/>
+      <c r="B7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="4"/>
-      <c r="B8" s="7" t="s">
+      <c r="A8" s="5"/>
+      <c r="B8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="4"/>
-      <c r="B9" s="7" t="s">
+      <c r="A9" s="5"/>
+      <c r="B9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="4"/>
-      <c r="B10" s="7" t="s">
+      <c r="A10" s="5"/>
+      <c r="B10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="4"/>
+      <c r="A11" s="5"/>
       <c r="B11" t="s">
         <v>12</v>
       </c>
@@ -734,31 +734,31 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="4"/>
+      <c r="A12" s="5"/>
       <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="5"/>
+      <c r="B13" t="s">
         <v>14</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>14</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D13" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="4"/>
-      <c r="B13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" t="s">
-        <v>13</v>
-      </c>
-    </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="4"/>
+      <c r="A14" s="5"/>
       <c r="B14" t="s">
         <v>20</v>
       </c>
@@ -770,7 +770,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="4"/>
+      <c r="A15" s="5"/>
       <c r="B15" t="s">
         <v>15</v>
       </c>
@@ -782,7 +782,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="6" t="s">
         <v>24</v>
       </c>
       <c r="B17" t="s">
@@ -796,7 +796,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="5"/>
+      <c r="A18" s="6"/>
       <c r="B18" t="s">
         <v>22</v>
       </c>
@@ -874,46 +874,46 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B31" t="s">
+      <c r="B31" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B32" t="s">
+      <c r="B32" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B33" t="s">
+      <c r="B33" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B34" t="s">
+      <c r="B34" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34" s="3" t="s">
         <v>11</v>
       </c>
     </row>
@@ -962,7 +962,7 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="6" t="s">
+      <c r="A41" s="7" t="s">
         <v>36</v>
       </c>
       <c r="B41" t="s">
@@ -976,7 +976,7 @@
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="6"/>
+      <c r="A42" s="7"/>
       <c r="B42" t="s">
         <v>26</v>
       </c>
@@ -988,7 +988,7 @@
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="6"/>
+      <c r="A43" s="7"/>
       <c r="C43" t="s">
         <v>29</v>
       </c>

</xml_diff>

<commit_message>
Change in Navbar (eSIF)
</commit_message>
<xml_diff>
--- a/Subject.xlsx
+++ b/Subject.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\nonisoft\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20112" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -137,7 +132,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -344,7 +339,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -379,7 +374,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -591,13 +586,15 @@
   <dimension ref="A1:D46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="7" width="42.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="42.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="42.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
@@ -611,7 +608,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>19</v>
       </c>
@@ -625,7 +622,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" t="s">
         <v>4</v>
@@ -637,7 +634,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" t="s">
         <v>5</v>
@@ -649,7 +646,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" t="s">
         <v>6</v>
@@ -661,7 +658,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" t="s">
         <v>7</v>
@@ -673,7 +670,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="3" t="s">
         <v>8</v>
@@ -685,7 +682,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="3" t="s">
         <v>9</v>
@@ -697,7 +694,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="3" t="s">
         <v>10</v>
@@ -709,7 +706,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="3" t="s">
         <v>11</v>
@@ -721,7 +718,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="B11" t="s">
         <v>12</v>
@@ -733,7 +730,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" t="s">
         <v>13</v>
@@ -745,7 +742,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" t="s">
         <v>14</v>
@@ -757,7 +754,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" t="s">
         <v>20</v>
@@ -769,7 +766,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" t="s">
         <v>15</v>
@@ -781,7 +778,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>24</v>
       </c>
@@ -795,7 +792,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" t="s">
         <v>22</v>
@@ -818,7 +815,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>3</v>
       </c>
@@ -829,7 +826,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>4</v>
       </c>
@@ -840,7 +837,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>5</v>
       </c>
@@ -851,7 +848,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>6</v>
       </c>
@@ -862,7 +859,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>7</v>
       </c>
@@ -873,7 +870,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B31" s="3" t="s">
         <v>8</v>
       </c>
@@ -884,7 +881,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B32" s="3" t="s">
         <v>9</v>
       </c>
@@ -895,7 +892,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B33" s="3" t="s">
         <v>10</v>
       </c>
@@ -906,7 +903,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B34" s="3" t="s">
         <v>11</v>
       </c>
@@ -917,7 +914,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>12</v>
       </c>
@@ -928,7 +925,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
         <v>13</v>
       </c>
@@ -939,7 +936,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>23</v>
       </c>
@@ -950,7 +947,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>15</v>
       </c>
@@ -961,7 +958,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
         <v>36</v>
       </c>
@@ -975,7 +972,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="7"/>
       <c r="B42" t="s">
         <v>26</v>
@@ -987,13 +984,13 @@
         <v>33</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="7"/>
       <c r="C43" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>30</v>
       </c>
@@ -1001,7 +998,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>31</v>
       </c>
@@ -1026,7 +1023,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1038,7 +1035,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>